<commit_message>
Update BOM and data sheets
</commit_message>
<xml_diff>
--- a/CADandPCB/PCB/BOM.xlsx
+++ b/CADandPCB/PCB/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MarkSherstan/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark Sherstan\Documents\GitHub Projects\GestureControlledRoboticArm_MecE653\CADandPCB\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA4577A-5D88-8B4B-89DD-CFEB98275EA7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30CA81AD-81C0-4ECD-B34C-D0FFCA1530F1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{B38504F5-FC03-014F-8501-1BD6B029E1B6}"/>
+    <workbookView xWindow="32460" yWindow="2385" windowWidth="11835" windowHeight="10725" xr2:uid="{B38504F5-FC03-014F-8501-1BD6B029E1B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="75">
   <si>
     <t>R1,R2,R3,R4,R5,R6,R7,R8</t>
   </si>
@@ -101,9 +102,6 @@
     <t>MPU-6050</t>
   </si>
   <si>
-    <t>MPU 6050 breakout!!</t>
-  </si>
-  <si>
     <t>Value</t>
   </si>
   <si>
@@ -167,9 +165,6 @@
     <t>https://www.digikey.ca/product-detail/en/ERJ-3EKF1001V/P1.00KHCT-ND</t>
   </si>
   <si>
-    <t>HC-05????</t>
-  </si>
-  <si>
     <t>https://www.digikey.ca/product-detail/en/ERJ-3EKF5101V/P5.10KHCT-ND</t>
   </si>
   <si>
@@ -218,9 +213,6 @@
     <t>Total Qty</t>
   </si>
   <si>
-    <t>% Extra</t>
-  </si>
-  <si>
     <t>ERJ-3EKF1002V</t>
   </si>
   <si>
@@ -242,9 +234,6 @@
     <t>https://www.digikey.ca/product-detail/en/dfrobot/SEN0142/1738-1070-ND/6588492</t>
   </si>
   <si>
-    <t>FSR</t>
-  </si>
-  <si>
     <t>Other</t>
   </si>
   <si>
@@ -252,6 +241,21 @@
   </si>
   <si>
     <t>https://www.digikey.ca/product-detail/en/trinamic-motion-control-gmbh/TMC2660-BOB/1460-1245-ND/8037672</t>
+  </si>
+  <si>
+    <t>x Extra</t>
+  </si>
+  <si>
+    <t>Rqd Qty</t>
+  </si>
+  <si>
+    <t>MPU 6050 Breakout</t>
+  </si>
+  <si>
+    <t>Stepper Motor Driver</t>
+  </si>
+  <si>
+    <t>Motor Controller / PDB</t>
   </si>
 </sst>
 </file>
@@ -261,7 +265,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -684,59 +688,57 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FC2C61D-DB80-FC4B-BCE7-85B9EE9E61B7}">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.5" style="4" customWidth="1"/>
-    <col min="2" max="2" width="9.83203125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="21.625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="4"/>
+    <col min="5" max="5" width="10.875" style="4"/>
     <col min="6" max="6" width="12" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="10" width="12" style="4" customWidth="1"/>
     <col min="11" max="11" width="82.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.83203125" style="4"/>
+    <col min="12" max="16384" width="10.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="9" customFormat="1" ht="19">
+    <row r="1" spans="1:11" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>26</v>
-      </c>
       <c r="J1" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K1" s="10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -744,10 +746,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="E2" s="3">
         <v>8</v>
@@ -763,17 +765,17 @@
         <v>40</v>
       </c>
       <c r="I2" s="2">
-        <f t="shared" ref="I2:I8" si="0">H2*F2</f>
+        <f t="shared" ref="I2:I11" si="0">H2*F2</f>
         <v>3.92</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -781,10 +783,10 @@
         <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E3" s="3">
         <v>1</v>
@@ -796,7 +798,7 @@
         <v>10</v>
       </c>
       <c r="H3" s="3">
-        <f t="shared" ref="H3:H11" si="1">E3*G3</f>
+        <f>E3*G3</f>
         <v>10</v>
       </c>
       <c r="I3" s="2">
@@ -804,13 +806,13 @@
         <v>0.98</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -818,10 +820,10 @@
         <v>8</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E4" s="3">
         <v>1</v>
@@ -833,7 +835,7 @@
         <v>10</v>
       </c>
       <c r="H4" s="3">
-        <f t="shared" si="1"/>
+        <f>E4*G4</f>
         <v>10</v>
       </c>
       <c r="I4" s="2">
@@ -841,13 +843,13 @@
         <v>0.98</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
@@ -855,10 +857,10 @@
         <v>9</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E5" s="3">
         <v>6</v>
@@ -867,24 +869,24 @@
         <v>9.8000000000000004E-2</v>
       </c>
       <c r="G5" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H5" s="3">
-        <f t="shared" si="1"/>
-        <v>48</v>
+        <f>E5*G5</f>
+        <v>42</v>
       </c>
       <c r="I5" s="2">
         <f t="shared" si="0"/>
-        <v>4.7040000000000006</v>
+        <v>4.1160000000000005</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
@@ -892,10 +894,10 @@
         <v>14</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E6" s="3">
         <v>3</v>
@@ -907,7 +909,7 @@
         <v>7</v>
       </c>
       <c r="H6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="H3:H11" si="1">E6*G6</f>
         <v>21</v>
       </c>
       <c r="I6" s="2">
@@ -915,13 +917,13 @@
         <v>0.98699999999999999</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
@@ -929,10 +931,10 @@
         <v>15</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E7" s="3">
         <v>1</v>
@@ -952,13 +954,13 @@
         <v>0.6</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
@@ -966,10 +968,10 @@
         <v>16</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E8" s="3">
         <v>1</v>
@@ -989,24 +991,24 @@
         <v>0.52</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E9" s="3">
         <v>2</v>
@@ -1022,28 +1024,28 @@
         <v>10</v>
       </c>
       <c r="I9" s="2">
-        <f t="shared" ref="I9:I10" si="2">H9*F9</f>
+        <f t="shared" si="0"/>
         <v>3.96</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K9" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E10" s="3">
         <v>1</v>
@@ -1059,28 +1061,28 @@
         <v>10</v>
       </c>
       <c r="I10" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>5.88</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>22</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E11" s="3">
         <v>1</v>
@@ -1096,46 +1098,46 @@
         <v>5</v>
       </c>
       <c r="I11" s="2">
-        <f>H11*F11</f>
+        <f t="shared" si="0"/>
         <v>55.039999999999992</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K11" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F13" s="2"/>
       <c r="H13" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I13" s="12">
         <f>SUM(I2:I11)</f>
-        <v>77.570999999999998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
+        <v>76.98299999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F14" s="2"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:11" ht="19">
+    <row r="15" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>2</v>
       </c>
       <c r="C15" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="10" t="s">
         <v>25</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>26</v>
       </c>
       <c r="E15" s="10" t="s">
         <v>3</v>
@@ -1143,9 +1145,9 @@
       <c r="F15" s="2"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="B16" s="4">
         <v>1</v>
@@ -1158,12 +1160,15 @@
         <v>14.47</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>73</v>
+      </c>
       <c r="B17" s="4">
         <v>2</v>
       </c>
@@ -1171,16 +1176,19 @@
         <v>12.05</v>
       </c>
       <c r="D17" s="2">
-        <f t="shared" ref="D17:D18" si="3">B17*C17</f>
+        <f t="shared" ref="D17:D18" si="2">B17*C17</f>
         <v>24.1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>74</v>
+      </c>
       <c r="B18" s="4">
         <v>1</v>
       </c>
@@ -1188,95 +1196,89 @@
         <v>30.13</v>
       </c>
       <c r="D18" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>30.13</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F19" s="2"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C20" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D20" s="15">
         <f>SUM(D16:D18)</f>
         <v>68.7</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C22" s="13"/>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" s="13"/>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C24" s="13"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>45</v>
       </c>
+      <c r="B25" s="13" t="s">
+        <v>52</v>
+      </c>
       <c r="C25" s="13"/>
       <c r="F25" s="8"/>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
+        <v>50</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>51</v>
+      </c>
       <c r="C27" s="13"/>
     </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B28" s="13" t="s">
-        <v>54</v>
-      </c>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C28" s="13"/>
     </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>15</v>
-      </c>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C29" s="13"/>
     </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>53</v>
-      </c>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C30" s="13"/>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C31" s="13"/>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C32" s="13"/>
     </row>
-    <row r="33" spans="3:3">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" s="13"/>
     </row>
-    <row r="34" spans="3:3">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34" s="13"/>
     </row>
   </sheetData>

</xml_diff>